<commit_message>
Last version of the mappings, updated used the new functionalities of MorphKGC
</commit_message>
<xml_diff>
--- a/MappingOCDS.xlsx
+++ b/MappingOCDS.xlsx
@@ -537,18 +537,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -643,55 +637,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -975,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1001,28 +990,28 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="19" t="s">
+      <c r="C3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="10" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1034,579 +1023,579 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:8" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="19" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="25" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:8" s="17" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="25" t="s">
+      <c r="C6" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="28" customFormat="1" ht="232.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="26" t="s">
+    <row r="7" spans="1:8" s="20" customFormat="1" ht="232.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="28" t="s">
+      <c r="C7" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="18" t="s">
+      <c r="C10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="10" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="127.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="19" t="s">
+      <c r="C11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="10" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F12" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="18" t="s">
+      <c r="F12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="18"/>
-      <c r="C13" s="18" t="s">
+      <c r="A13" s="10"/>
+      <c r="C13" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
+    <row r="15" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="10" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="10" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="19" t="s">
+      <c r="F17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="30" customFormat="1" ht="189" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="30" t="s">
+    <row r="18" spans="1:8" s="22" customFormat="1" ht="189" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="30" t="s">
+      <c r="C18" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="F18" s="30" t="s">
+      <c r="F18" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="H18" s="30" t="s">
+      <c r="H18" s="22" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="F19" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="38" t="s">
+      <c r="F19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="14" t="s">
+    <row r="20" spans="1:8" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="39" t="s">
+      <c r="E20" s="31" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:8" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
+    <row r="22" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="14" t="s">
+    <row r="23" spans="1:8" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="18" t="s">
+    <row r="24" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="19" t="s">
+      <c r="F24" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="H24" s="18" t="s">
+      <c r="H24" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="18" t="s">
+    <row r="25" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G25" s="19" t="s">
+      <c r="F25" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:8" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="21" t="s">
+    <row r="27" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="F27" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="G27" s="32" t="s">
+      <c r="F27" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="H27" s="32" t="s">
+      <c r="H27" s="24" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="34" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="33" t="s">
+    <row r="28" spans="1:8" s="26" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="E28" s="34" t="s">
+      <c r="E28" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="21" t="s">
+    <row r="29" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="32" t="s">
+      <c r="D29" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E29" s="32" t="s">
+      <c r="E29" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="G29" s="32" t="s">
+      <c r="F29" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="H29" s="32" t="s">
+      <c r="H29" s="24" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="34" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="33" t="s">
+    <row r="30" spans="1:8" s="26" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="E30" s="34" t="s">
+      <c r="E30" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="18" t="s">
+    <row r="31" spans="1:8" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="18" t="s">
+      <c r="C31" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="24" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G33" s="7" t="s">
+      <c r="F33" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G33" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="H33" s="7" t="s">
+      <c r="H33" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="I33" s="7" t="s">
+      <c r="I33" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="J33" s="7" t="s">
+      <c r="J33" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="K33" s="7" t="s">
+      <c r="K33" s="29" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:11" s="26" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="21" t="s">
+    <row r="35" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G35" s="18" t="s">
+      <c r="E35" s="10"/>
+      <c r="F35" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G35" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="H35" s="18" t="s">
+      <c r="H35" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
-    </row>
-    <row r="36" spans="1:11" s="37" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="36" t="s">
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+    </row>
+    <row r="36" spans="1:11" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="G36" s="18" t="s">
+      <c r="E36" s="10"/>
+      <c r="F36" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G36" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="H36" s="18" t="s">
+      <c r="H36" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-    </row>
-    <row r="37" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+    </row>
+    <row r="37" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="4" t="s">
+      <c r="H37" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="26" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="27" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1614,43 +1603,43 @@
       <c r="A39" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="8" t="s">
+    <row r="40" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="8" t="s">
+    <row r="41" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1671,9 +1660,11 @@
     <hyperlink ref="D36" r:id="rId13" location="periodEndDate"/>
     <hyperlink ref="D35" r:id="rId14" location="periodEndDate"/>
     <hyperlink ref="G25" r:id="rId15" location="hasContractPeriod"/>
+    <hyperlink ref="D38" r:id="rId16" location="legalName"/>
+    <hyperlink ref="G37" r:id="rId17" location="isProcuringEntityFor"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
-  <legacyDrawing r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <legacyDrawing r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>